<commit_message>
f2v cal through sn 5
</commit_message>
<xml_diff>
--- a/Saves/F2V_Cal20171203.xlsx
+++ b/Saves/F2V_Cal20171203.xlsx
@@ -4,26 +4,27 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary V4" sheetId="2" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Data!#REF!</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Freq, Hz</t>
   </si>
@@ -71,6 +72,9 @@
   </si>
   <si>
     <t>P_V4_NT(3)</t>
+  </si>
+  <si>
+    <t>dropout, vrms</t>
   </si>
 </sst>
 </file>
@@ -141,6 +145,1099 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>F2V Board Calibration</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SN0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$F$2:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.71799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8979999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SN1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$G$2:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.72899999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.456</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SN2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$H$2:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.69199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92200000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SN3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$I$2:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.861</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SN4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$J$2:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.71399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SN5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$K$2:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.70699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.94199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.409</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.78</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.01</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SN6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>650</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$L$2:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="207832312"/>
+        <c:axId val="207835056"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="207832312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequency, Hz</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="207835056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="207835056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="207832312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -293,7 +1390,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -329,7 +1426,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$10</c:f>
+              <c:f>Data!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
@@ -355,11 +1452,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="493073080"/>
-        <c:axId val="493078960"/>
+        <c:axId val="202932144"/>
+        <c:axId val="202934104"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="493073080"/>
+        <c:axId val="202932144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -476,12 +1573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493078960"/>
+        <c:crossAx val="202934104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="493078960"/>
+        <c:axId val="202934104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -594,7 +1691,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="493073080"/>
+        <c:crossAx val="202932144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -643,7 +1740,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -724,7 +1821,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Data!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -755,7 +1852,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -791,7 +1888,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$10</c:f>
+              <c:f>Data!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -832,7 +1929,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Data!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -863,7 +1960,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -899,7 +1996,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$10</c:f>
+              <c:f>Data!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -940,7 +2037,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Data!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -973,7 +2070,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1009,10 +2106,37 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$10</c:f>
+              <c:f>Data!$H$2:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.69199999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.92200000000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3819999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.839</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.96</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1023,7 +2147,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Data!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1056,7 +2180,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1092,10 +2216,37 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$10</c:f>
+              <c:f>Data!$I$2:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.70199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93600000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.861</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.54</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.99</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1106,7 +2257,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Data!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1139,7 +2290,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1175,10 +2326,37 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$10</c:f>
+              <c:f>Data!$J$2:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.71399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.05</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1189,7 +2367,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>Data!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1222,7 +2400,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1258,7 +2436,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$10</c:f>
+              <c:f>Data!$K$2:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1299,7 +2477,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>Data!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1336,7 +2514,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Data!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1372,7 +2550,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$10</c:f>
+              <c:f>Data!$L$2:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1389,8 +2567,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="504389168"/>
-        <c:axId val="504386816"/>
+        <c:axId val="202932928"/>
+        <c:axId val="202934496"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -1402,7 +2580,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$M$1</c15:sqref>
+                          <c15:sqref>Data!$M$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1442,7 +2620,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$A$2:$A$10</c15:sqref>
+                          <c15:sqref>Data!$A$2:$A$10</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1484,7 +2662,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Sheet1!$M$2:$M$10</c15:sqref>
+                          <c15:sqref>Data!$M$2:$M$10</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1501,7 +2679,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="504389168"/>
+        <c:axId val="202932928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,12 +2797,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="504386816"/>
+        <c:crossAx val="202934496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="504386816"/>
+        <c:axId val="202934496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1744,7 +2922,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="504389168"/>
+        <c:crossAx val="202932928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1905,6 +3083,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2937,7 +4155,561 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="64" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8679656" cy="6298406"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3291,8 +5063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3301,9 +5073,7 @@
     <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="4.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -3374,6 +5144,15 @@
       <c r="G2" s="1">
         <v>0.72899999999999998</v>
       </c>
+      <c r="H2" s="1">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.71399999999999997</v>
+      </c>
       <c r="K2" s="1">
         <v>0.70699999999999996</v>
       </c>
@@ -3405,6 +5184,15 @@
       <c r="G3" s="1">
         <v>0.97299999999999998</v>
       </c>
+      <c r="H3" s="1">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.95199999999999996</v>
+      </c>
       <c r="K3" s="1">
         <v>0.94199999999999995</v>
       </c>
@@ -3436,6 +5224,15 @@
       <c r="G4" s="1">
         <v>1.456</v>
       </c>
+      <c r="H4" s="1">
+        <v>1.3819999999999999</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1.43</v>
+      </c>
       <c r="K4" s="1">
         <v>1.409</v>
       </c>
@@ -3469,6 +5266,15 @@
       <c r="G5" s="1">
         <v>1.93</v>
       </c>
+      <c r="H5" s="1">
+        <v>1.839</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.861</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.9</v>
+      </c>
       <c r="K5" s="1">
         <v>1.8720000000000001</v>
       </c>
@@ -3500,6 +5306,15 @@
       <c r="G6" s="1">
         <v>2.17</v>
       </c>
+      <c r="H6" s="1">
+        <v>2.06</v>
+      </c>
+      <c r="I6" s="1">
+        <v>2.08</v>
+      </c>
+      <c r="J6" s="1">
+        <v>2.12</v>
+      </c>
       <c r="K6" s="1">
         <v>2.1</v>
       </c>
@@ -3531,6 +5346,15 @@
       <c r="G7" s="1">
         <v>2.41</v>
       </c>
+      <c r="H7" s="1">
+        <v>2.29</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2.36</v>
+      </c>
       <c r="K7" s="1">
         <v>2.33</v>
       </c>
@@ -3562,6 +5386,15 @@
       <c r="G8" s="1">
         <v>2.64</v>
       </c>
+      <c r="H8" s="1">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="I8" s="1">
+        <v>2.54</v>
+      </c>
+      <c r="J8" s="1">
+        <v>2.59</v>
+      </c>
       <c r="K8" s="1">
         <v>2.5499999999999998</v>
       </c>
@@ -3595,6 +5428,15 @@
       <c r="G9" s="1">
         <v>2.88</v>
       </c>
+      <c r="H9" s="1">
+        <v>2.74</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2.76</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2.82</v>
+      </c>
       <c r="K9" s="1">
         <v>2.78</v>
       </c>
@@ -3625,6 +5467,15 @@
       </c>
       <c r="G10" s="1">
         <v>3.12</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3.05</v>
       </c>
       <c r="K10" s="1">
         <v>3.01</v>
@@ -3654,9 +5505,18 @@
         <f>INDEX(LINEST($N$2:$N$10,G$2:G$10^{1,2},FALSE,FALSE),3)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="H13" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,H$2:H$10^{1,2},FALSE,FALSE),3)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,I$2:I$10^{1,2},FALSE,FALSE),3)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,J$2:J$10^{1,2},FALSE,FALSE),3)</f>
+        <v>0</v>
+      </c>
       <c r="K13" s="2">
         <f>INDEX(LINEST($N$2:$N$10,K$2:K$10^{1,2},FALSE,FALSE),3)</f>
         <v>0</v>
@@ -3677,9 +5537,18 @@
         <f>INDEX(LINEST($N$2:$N$10,G$2:G$10^{1,2},FALSE,FALSE),2)</f>
         <v>12276.075278443672</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="H14" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,H$2:H$10^{1,2},FALSE,FALSE),2)</f>
+        <v>12913.980695566312</v>
+      </c>
+      <c r="I14" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,I$2:I$10^{1,2},FALSE,FALSE),2)</f>
+        <v>12700.548566313257</v>
+      </c>
+      <c r="J14" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,J$2:J$10^{1,2},FALSE,FALSE),2)</f>
+        <v>12477.470633810395</v>
+      </c>
       <c r="K14" s="2">
         <f>INDEX(LINEST($N$2:$N$10,K$2:K$10^{1,2},FALSE,FALSE),2)</f>
         <v>12617.500101766993</v>
@@ -3700,9 +5569,18 @@
         <f>INDEX(LINEST($N$2:$N$10,G$2:G$10^{1,2},FALSE,FALSE),1)</f>
         <v>76.042553979691533</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="H15" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,H$2:H$10^{1,2},FALSE,FALSE),1)</f>
+        <v>86.515992795181035</v>
+      </c>
+      <c r="I15" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,I$2:I$10^{1,2},FALSE,FALSE),1)</f>
+        <v>116.2825951519487</v>
+      </c>
+      <c r="J15" s="2">
+        <f>INDEX(LINEST($N$2:$N$10,J$2:J$10^{1,2},FALSE,FALSE),1)</f>
+        <v>101.82059256467288</v>
+      </c>
       <c r="K15" s="2">
         <f>INDEX(LINEST($N$2:$N$10,K$2:K$10^{1,2},FALSE,FALSE),1)</f>
         <v>116.48400617638146</v>
@@ -3715,35 +5593,50 @@
       <c r="M16" s="1"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>150</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.05</v>
+      </c>
       <c r="M17" s="1"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M18" s="1"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M19" s="1"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M21" s="1"/>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M22" s="1"/>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="M23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24"/>

</xml_diff>